<commit_message>
fix error for tuples of 2
</commit_message>
<xml_diff>
--- a/output/fRAT_check_2_solution_True.xlsx
+++ b/output/fRAT_check_2_solution_True.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rejna\Work_only_here\Miscellaneous\rakshitha\output\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBEF94E-782E-4FE9-8F7E-18F21B241848}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -553,8 +559,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -617,6 +623,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -663,7 +677,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -695,9 +709,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -729,6 +761,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -904,14 +954,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.90625" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" customWidth="1"/>
+    <col min="3" max="3" width="22.08984375" customWidth="1"/>
+    <col min="4" max="4" width="22.26953125" customWidth="1"/>
+    <col min="5" max="5" width="23.36328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -931,7 +988,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -948,7 +1005,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -965,7 +1022,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -982,7 +1039,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -993,7 +1050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1010,7 +1067,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1021,7 +1078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1038,7 +1095,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1055,7 +1112,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1072,7 +1129,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1089,7 +1146,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1106,7 +1163,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1123,7 +1180,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1140,7 +1197,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1157,7 +1214,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1174,7 +1231,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1185,7 +1242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1196,7 +1253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1213,7 +1270,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1230,7 +1287,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1247,7 +1304,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1264,7 +1321,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1281,7 +1338,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1298,7 +1355,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1309,7 +1366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1326,7 +1383,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1343,7 +1400,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1354,7 +1411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1371,7 +1428,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1382,7 +1439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1399,7 +1456,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1416,7 +1473,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -1433,7 +1490,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1450,7 +1507,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1467,7 +1524,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -1484,7 +1541,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -1501,7 +1558,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -1512,7 +1569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -1529,7 +1586,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -1540,7 +1597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -1557,7 +1614,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -1574,7 +1631,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -1591,7 +1648,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -1608,7 +1665,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -1625,7 +1682,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -1636,7 +1693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -1653,7 +1710,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -1670,7 +1727,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -1687,7 +1744,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>54</v>
       </c>
@@ -1704,7 +1761,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -1715,7 +1772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -1732,7 +1789,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>57</v>
       </c>
@@ -1749,7 +1806,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -1766,7 +1823,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>59</v>
       </c>
@@ -1783,7 +1840,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -1800,7 +1857,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>61</v>
       </c>
@@ -1811,7 +1868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>62</v>
       </c>
@@ -1828,7 +1885,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -1845,7 +1902,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>64</v>
       </c>
@@ -1862,7 +1919,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>65</v>
       </c>
@@ -1879,7 +1936,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>66</v>
       </c>
@@ -1890,7 +1947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>67</v>
       </c>
@@ -1901,7 +1958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>68</v>
       </c>
@@ -1918,7 +1975,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>69</v>
       </c>
@@ -1929,7 +1986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>70</v>
       </c>
@@ -1940,7 +1997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>71</v>
       </c>
@@ -1951,7 +2008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>72</v>
       </c>
@@ -1968,7 +2025,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>73</v>
       </c>
@@ -1979,7 +2036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>74</v>
       </c>
@@ -1996,7 +2053,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>75</v>
       </c>
@@ -2013,7 +2070,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>76</v>
       </c>
@@ -2030,7 +2087,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>77</v>
       </c>
@@ -2041,7 +2098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F74" t="s">
         <v>177</v>
       </c>

</xml_diff>